<commit_message>
updated inference time table
</commit_message>
<xml_diff>
--- a/experiments/combination-overhead/InferenceTime.xlsx
+++ b/experiments/combination-overhead/InferenceTime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yannic/repositories/DNN-Repair/experiments/combination-overhead/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBC51B3-E102-D643-8BE1-44D96206EF5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118BC54C-65E0-3A42-8835-E3C56FBE5E24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{3DF0A38D-930F-5648-AD79-5307487A5539}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="E20" sqref="A17:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,7 +478,7 @@
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -512,7 +512,7 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -562,7 +562,7 @@
       <c r="D8" s="3">
         <v>0.41547360000000999</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <f>D8/D$5</f>
         <v>1.0768089596198398</v>
       </c>
@@ -580,7 +580,7 @@
       <c r="D9" s="3">
         <v>0.41552450000000901</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <f>D9/D$5</f>
         <v>1.0769408803388545</v>
       </c>
@@ -598,7 +598,7 @@
       <c r="D10" s="3">
         <v>0.41555240000000798</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <f>D10/D$5</f>
         <v>1.0770131905168592</v>
       </c>
@@ -629,7 +629,7 @@
       <c r="D13" s="3">
         <v>3.2419277000000202</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <f>D13/D$5</f>
         <v>8.4023071352780967</v>
       </c>
@@ -647,7 +647,7 @@
       <c r="D14" s="3">
         <v>3.2419752000000099</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <f>D14/D$5</f>
         <v>8.4024302440040692</v>
       </c>
@@ -665,7 +665,7 @@
       <c r="D15" s="3">
         <v>3.24200000000002</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <f>D15/D$5</f>
         <v>8.4024945197178784</v>
       </c>
@@ -696,7 +696,7 @@
       <c r="D18" s="3">
         <v>1.3453532000000099</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <f>D18/D$5</f>
         <v>3.4868361783112047</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="D19" s="3">
         <v>1.3453725999999999</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <f>D19/D$5</f>
         <v>3.486886458506639</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="D20" s="3">
         <v>1.3453603999999999</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <f>D20/D$5</f>
         <v>3.4868548390022776</v>
       </c>

</xml_diff>